<commit_message>
Modificacion de proyecto Ui
</commit_message>
<xml_diff>
--- a/data/adjacency_matrix.xlsx
+++ b/data/adjacency_matrix.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,6 +490,26 @@
           <t>10</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -505,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -523,6 +543,18 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -540,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -558,6 +590,18 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -575,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -593,6 +637,18 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -610,7 +666,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -628,21 +684,33 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -663,6 +731,18 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -700,6 +780,18 @@
       <c r="K7" t="n">
         <v>0</v>
       </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -735,6 +827,18 @@
       <c r="K8" t="n">
         <v>0</v>
       </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -770,6 +874,18 @@
       <c r="K9" t="n">
         <v>0</v>
       </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -805,6 +921,18 @@
       <c r="K10" t="n">
         <v>0</v>
       </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -840,6 +968,18 @@
       <c r="K11" t="n">
         <v>0</v>
       </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -873,6 +1013,206 @@
         <v>0</v>
       </c>
       <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -887,7 +1227,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -951,28 +1291,42 @@
           <t>10</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>93</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
+      <c r="B2" t="n">
+        <v>66</v>
+      </c>
+      <c r="C2" t="n">
+        <v>95</v>
+      </c>
+      <c r="D2" t="n">
+        <v>45</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -992,28 +1346,34 @@
       <c r="K2" t="n">
         <v>0</v>
       </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+      <c r="A3" t="n">
+        <v>66</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
+      <c r="C3" t="n">
+        <v>83</v>
+      </c>
+      <c r="D3" t="n">
+        <v>51</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -1033,28 +1393,34 @@
       <c r="K3" t="n">
         <v>0</v>
       </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>93</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+      <c r="A4" t="n">
+        <v>95</v>
+      </c>
+      <c r="B4" t="n">
+        <v>83</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+      <c r="D4" t="n">
+        <v>68</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -1074,28 +1440,34 @@
       <c r="K4" t="n">
         <v>0</v>
       </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+      <c r="A5" t="n">
+        <v>45</v>
+      </c>
+      <c r="B5" t="n">
+        <v>51</v>
+      </c>
+      <c r="C5" t="n">
+        <v>68</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -1113,21 +1485,33 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -1148,6 +1532,18 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1185,6 +1581,18 @@
       <c r="K7" t="n">
         <v>0</v>
       </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1220,6 +1628,18 @@
       <c r="K8" t="n">
         <v>0</v>
       </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1255,6 +1675,18 @@
       <c r="K9" t="n">
         <v>0</v>
       </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1290,6 +1722,18 @@
       <c r="K10" t="n">
         <v>0</v>
       </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1325,6 +1769,18 @@
       <c r="K11" t="n">
         <v>0</v>
       </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1358,6 +1814,206 @@
         <v>0</v>
       </c>
       <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>